<commit_message>
flood risk class updates
</commit_message>
<xml_diff>
--- a/Treatment-Control-Assignment/recurrence_Impact_calc_example_4Sri.xlsx
+++ b/Treatment-Control-Assignment/recurrence_Impact_calc_example_4Sri.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Desktop\C2S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srilakshmi/Desktop/Thesis/Treatment-Control-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17F1D098-EFE0-4AD1-9375-D0B9452AA83F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EEF931-2611-0944-B801-210CE41327BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{3B35F228-9433-4074-9481-44D00142EA24}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26460" windowHeight="17060" xr2:uid="{3B35F228-9433-4074-9481-44D00142EA24}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Recurrence Map - Population" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>2yr</t>
   </si>
@@ -48,30 +48,47 @@
     <t>20yr</t>
   </si>
   <si>
-    <t>impact</t>
-  </si>
-  <si>
-    <t>marginal impact</t>
-  </si>
-  <si>
-    <t>marginal impact per year</t>
-  </si>
-  <si>
-    <t>average impact per year</t>
-  </si>
-  <si>
-    <t>population</t>
-  </si>
-  <si>
-    <t>East gonja</t>
+    <t>East Gonja</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t>Marginal impact</t>
+  </si>
+  <si>
+    <t>Marginal impact per year</t>
+  </si>
+  <si>
+    <t>Average impact per year</t>
+  </si>
+  <si>
+    <t>0yr</t>
+  </si>
+  <si>
+    <t>15yr</t>
+  </si>
+  <si>
+    <t>Accra Metropolis</t>
+  </si>
+  <si>
+    <t>Ada West</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,8 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,20 +433,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EBBE5B-4AE5-4F1C-B1F6-F63C34321289}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
@@ -441,10 +459,13 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D2">
         <v>2</v>
       </c>
@@ -455,15 +476,18 @@
         <v>10</v>
       </c>
       <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -478,12 +502,15 @@
         <v>5000</v>
       </c>
       <c r="G3">
+        <v>17000</v>
+      </c>
+      <c r="H3">
         <v>30000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <f>D3-C3</f>
@@ -499,19 +526,23 @@
       </c>
       <c r="G4">
         <f>G3-F3</f>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>12000</v>
+      </c>
+      <c r="H4">
+        <f>H3-G3</f>
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <f>D4/D2</f>
         <v>50</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:G5" si="0">E4/E2</f>
+        <f t="shared" ref="E5:H5" si="0">E4/E2</f>
         <v>180</v>
       </c>
       <c r="F5">
@@ -520,16 +551,224 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+        <v>800</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <f>SUM(D5:H5)</f>
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>356</v>
+      </c>
+      <c r="F9">
+        <v>807</v>
+      </c>
+      <c r="G9">
+        <v>1071</v>
+      </c>
+      <c r="H9">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <f>D9-C9</f>
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <f>E9-D9</f>
+        <v>315</v>
+      </c>
+      <c r="F10">
+        <f>F9-E9</f>
+        <v>451</v>
+      </c>
+      <c r="G10">
+        <f>G9-F9</f>
+        <v>264</v>
+      </c>
+      <c r="H10">
+        <f>H9-G9</f>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
-        <f>SUM(D5:G5)</f>
-        <v>1880</v>
+      <c r="D11">
+        <f>D10/D8</f>
+        <v>20.5</v>
+      </c>
+      <c r="E11">
+        <f>E10/E8</f>
+        <v>63</v>
+      </c>
+      <c r="F11">
+        <f>F10/F8</f>
+        <v>45.1</v>
+      </c>
+      <c r="G11">
+        <f>G10/G8</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H11">
+        <f>H10/H8</f>
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <f>SUM(D11:H11)</f>
+        <v>156.44999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+      <c r="H14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>384</v>
+      </c>
+      <c r="F15">
+        <v>658</v>
+      </c>
+      <c r="G15">
+        <v>801</v>
+      </c>
+      <c r="H15">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f>D15-C15</f>
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <f>E15-D15</f>
+        <v>366</v>
+      </c>
+      <c r="F16">
+        <f>F15-E15</f>
+        <v>274</v>
+      </c>
+      <c r="G16">
+        <f>G15-F15</f>
+        <v>143</v>
+      </c>
+      <c r="H16">
+        <f>H15-G15</f>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <f>D16/D14</f>
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <f>E16/E14</f>
+        <v>73.2</v>
+      </c>
+      <c r="F17">
+        <f>F16/F14</f>
+        <v>27.4</v>
+      </c>
+      <c r="G17">
+        <f>G16/G14</f>
+        <v>9.5333333333333332</v>
+      </c>
+      <c r="H17">
+        <f>H16/H14</f>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1">
+        <f>SUM(D17:H17)</f>
+        <v>128.53333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>